<commit_message>
Added test data for pack 4
</commit_message>
<xml_diff>
--- a/ATPs/ATP-01/01_Accumulator_Verification.xlsx
+++ b/ATPs/ATP-01/01_Accumulator_Verification.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
     <sheet name="Pack 1" sheetId="1" r:id="rId2"/>
     <sheet name="Pack 2" sheetId="7" r:id="rId3"/>
+    <sheet name="Pack 4" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Pack 2'!$A$1:$F$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Pack 4'!$A$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="59">
-  <si>
-    <t>System current:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="61">
   <si>
     <t>Measurement point 1</t>
   </si>
@@ -40,9 +39,6 @@
     <t>Measurement point 2</t>
   </si>
   <si>
-    <t>Amps</t>
-  </si>
-  <si>
     <t>Voltage (mV)</t>
   </si>
   <si>
@@ -206,6 +202,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Test:</t>
+  </si>
+  <si>
+    <t>Current:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack: </t>
   </si>
 </sst>
 </file>
@@ -251,16 +259,122 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -720,7 +834,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -732,49 +846,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="E1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4">
-        <f>(D4*1000)/$C$1</f>
+        <f>(D4*1000)/$D$1</f>
         <v>0</v>
       </c>
       <c r="F4">
@@ -783,17 +903,17 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5">
-        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$C$1</f>
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
         <v>0</v>
       </c>
       <c r="F5">
@@ -802,13 +922,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6">
@@ -821,13 +941,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7">
@@ -840,13 +960,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8">
@@ -859,13 +979,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9">
@@ -878,13 +998,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10">
@@ -897,13 +1017,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11">
@@ -916,13 +1036,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12">
@@ -935,13 +1055,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13">
@@ -954,13 +1074,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14">
@@ -973,13 +1093,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15">
@@ -992,13 +1112,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16">
@@ -1011,13 +1131,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17">
@@ -1030,13 +1150,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18">
@@ -1044,18 +1164,18 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19">
@@ -1063,18 +1183,18 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20">
@@ -1082,18 +1202,18 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21">
@@ -1101,18 +1221,18 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22">
@@ -1120,18 +1240,18 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23">
@@ -1139,18 +1259,18 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24">
@@ -1158,18 +1278,18 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25">
@@ -1177,18 +1297,18 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26">
@@ -1196,18 +1316,18 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27">
@@ -1215,36 +1335,37 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
         <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29">
@@ -1252,18 +1373,18 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30">
@@ -1271,18 +1392,18 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31">
@@ -1290,18 +1411,18 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32">
@@ -1309,18 +1430,18 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33">
@@ -1328,18 +1449,18 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34">
@@ -1347,18 +1468,18 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
         <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35">
@@ -1366,18 +1487,18 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36">
@@ -1385,18 +1506,18 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
         <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37">
@@ -1404,18 +1525,18 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38">
@@ -1423,18 +1544,18 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39">
@@ -1442,17 +1563,17 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1465,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1478,34 +1599,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="E1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,7 +1652,7 @@
         <v>1.53</v>
       </c>
       <c r="E4">
-        <f>(D4*1000)/$C$1</f>
+        <f>(D4*1000)/$D$1</f>
         <v>76.5</v>
       </c>
       <c r="F4">
@@ -1550,7 +1677,7 @@
         <v>1.31</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$C$1</f>
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
         <v>65.5</v>
       </c>
       <c r="F5">
@@ -2103,6 +2230,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28" t="str">
@@ -2365,12 +2493,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2383,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2396,51 +2524,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="E1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>0.752</v>
       </c>
       <c r="E4">
-        <f>(D4*1000)/$C$1</f>
+        <f>(D4*1000)/$D$1</f>
         <v>37.6</v>
       </c>
       <c r="F4">
@@ -2449,19 +2583,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>5.1639999999999997</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$C$1</f>
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
         <v>258.2</v>
       </c>
       <c r="F5">
@@ -2470,13 +2604,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -2491,13 +2625,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
         <v>0.35199999999999998</v>
@@ -2512,13 +2646,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>1.1930000000000001</v>
@@ -2533,13 +2667,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2">
         <v>6.702</v>
@@ -2554,13 +2688,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2">
         <v>1.0069999999999999</v>
@@ -2575,13 +2709,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
         <v>1.4890000000000001</v>
@@ -2596,13 +2730,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2">
         <v>4.0110000000000001</v>
@@ -2617,13 +2751,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2">
         <v>2.0419999999999998</v>
@@ -2638,13 +2772,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
         <v>0.622</v>
@@ -2659,13 +2793,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2">
         <v>0.27700000000000002</v>
@@ -2680,13 +2814,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
         <v>0.9</v>
@@ -2701,13 +2835,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="2">
         <v>1.651</v>
@@ -2722,13 +2856,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2">
         <v>9.4E-2</v>
@@ -2738,18 +2872,18 @@
         <v>4.7</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <v>0.10199999999999999</v>
@@ -2759,18 +2893,18 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2">
         <v>9.8000000000000004E-2</v>
@@ -2780,18 +2914,18 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2">
         <v>0.1</v>
@@ -2801,18 +2935,18 @@
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="2">
         <v>0.10299999999999999</v>
@@ -2822,18 +2956,18 @@
         <v>5.15</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2">
         <v>0.108</v>
@@ -2843,18 +2977,18 @@
         <v>5.4</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2">
         <v>0.23599999999999999</v>
@@ -2864,18 +2998,18 @@
         <v>11.8</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="2">
         <v>0.30499999999999999</v>
@@ -2885,18 +3019,18 @@
         <v>15.25</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <v>0.28100000000000003</v>
@@ -2906,18 +3040,18 @@
         <v>14.05</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="2">
         <v>0.42199999999999999</v>
@@ -2927,38 +3061,39 @@
         <v>21.1</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="2">
         <v>0.105</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.25</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
         <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
       </c>
       <c r="D29" s="2">
         <v>3.4820000000000002</v>
@@ -2968,18 +3103,18 @@
         <v>174.1</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30">
@@ -2987,18 +3122,18 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31">
@@ -3006,18 +3141,18 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" s="2">
         <v>0.42699999999999999</v>
@@ -3027,18 +3162,18 @@
         <v>21.35</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="2">
         <v>3.5000000000000003E-2</v>
@@ -3048,18 +3183,18 @@
         <v>1.75</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D34" s="2">
         <v>5.7000000000000002E-2</v>
@@ -3069,18 +3204,18 @@
         <v>2.85</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
         <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
       </c>
       <c r="D35" s="2">
         <v>6.5000000000000002E-2</v>
@@ -3090,18 +3225,18 @@
         <v>3.25</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D36" s="2">
         <v>6.0549999999999997</v>
@@ -3111,18 +3246,18 @@
         <v>302.75</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
         <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
       </c>
       <c r="D37" s="2">
         <v>6.2E-2</v>
@@ -3132,18 +3267,18 @@
         <v>3.1</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="2">
         <v>0.29899999999999999</v>
@@ -3153,18 +3288,18 @@
         <v>14.95</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" s="2">
         <v>0.19900000000000001</v>
@@ -3174,7 +3309,828 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E4">
+        <f>(D4*1000)/$D$1</f>
+        <v>22.35</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.157</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
+        <v>107.85</v>
+      </c>
+      <c r="F5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>41.55</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.407</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>120.35</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>36.25</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.7370000000000001</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>86.85</v>
+      </c>
+      <c r="F10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.593</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>79.650000000000006</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.83</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>191.5</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>29.55</v>
+      </c>
+      <c r="F13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.661</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>83.05</v>
+      </c>
+      <c r="F14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>73.55</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>120.25</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.316</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>15.8</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.214</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>19.3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>8.85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>151.25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>20.45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5.4050000000000002</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>270.25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>5.3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.153</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>7.65</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3184,7 +4140,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added pack 3 data
</commit_message>
<xml_diff>
--- a/ATPs/ATP-01/01_Accumulator_Verification.xlsx
+++ b/ATPs/ATP-01/01_Accumulator_Verification.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
     <sheet name="Pack 1" sheetId="1" r:id="rId2"/>
     <sheet name="Pack 2" sheetId="7" r:id="rId3"/>
-    <sheet name="Pack 4" sheetId="8" r:id="rId4"/>
+    <sheet name="Pack 3" sheetId="9" r:id="rId4"/>
+    <sheet name="Pack 4" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Pack 2'!$A$1:$F$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Pack 4'!$A$1:$E$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Pack 3'!$A$1:$F$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Pack 4'!$A$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="61">
   <si>
     <t>Measurement point 1</t>
   </si>
@@ -274,7 +276,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -362,186 +364,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -834,7 +656,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1568,12 +1390,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1586,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2493,12 +2315,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2512,7 +2334,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3314,12 +3136,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3332,7 +3154,832 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="E4">
+        <f>(D4*1000)/$D$1</f>
+        <v>20.85</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
+        <v>65</v>
+      </c>
+      <c r="F5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.46</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.9689999999999999</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>198.45</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7.0229999999999997</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>351.15</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6.0129999999999999</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>300.64999999999998</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.84</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>397.5</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.601</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>330.05</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.9420000000000002</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>147.1</v>
+      </c>
+      <c r="F13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3.7349999999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>186.75</v>
+      </c>
+      <c r="F14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2.0680000000000001</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>103.4</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.77</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>138.5</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.351</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>67.55</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.221</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>11.05</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>13.45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>4.05</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>19.2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.108</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.4369999999999998</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>171.85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3.206</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>160.30000000000001</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>7.1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>17.95</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5.617</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>280.85000000000002</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.128</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -4135,12 +4782,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>F4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Pack 2 with a new test
</commit_message>
<xml_diff>
--- a/ATPs/ATP-01/01_Accumulator_Verification.xlsx
+++ b/ATPs/ATP-01/01_Accumulator_Verification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
@@ -2334,7 +2334,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2414,11 +2414,11 @@
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>5.1639999999999997</v>
+        <v>0.79800000000000004</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
-        <v>258.2</v>
+        <v>39.9</v>
       </c>
       <c r="F5">
         <v>150</v>
@@ -2435,11 +2435,11 @@
         <v>21</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>1.296</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>64.8</v>
       </c>
       <c r="F6">
         <v>150</v>
@@ -2498,11 +2498,11 @@
         <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>6.702</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>335.1</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>150</v>
@@ -2519,11 +2519,11 @@
         <v>25</v>
       </c>
       <c r="D10" s="2">
-        <v>1.0069999999999999</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>50.349999999999994</v>
+        <v>27.2</v>
       </c>
       <c r="F10">
         <v>150</v>
@@ -2540,11 +2540,11 @@
         <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>1.4890000000000001</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>74.45</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>150</v>
@@ -2561,11 +2561,11 @@
         <v>27</v>
       </c>
       <c r="D12" s="2">
-        <v>4.0110000000000001</v>
+        <v>1.88</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>200.55</v>
+        <v>94</v>
       </c>
       <c r="F12">
         <v>150</v>
@@ -3154,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3277,11 +3277,11 @@
         <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>3.9689999999999999</v>
+        <v>5.8360000000000003</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>198.45</v>
+        <v>291.8</v>
       </c>
       <c r="F7">
         <v>150</v>
@@ -3298,11 +3298,11 @@
         <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>7.0229999999999997</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>351.15</v>
+        <v>44.1</v>
       </c>
       <c r="F8">
         <v>150</v>
@@ -3319,11 +3319,11 @@
         <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>6.0129999999999999</v>
+        <v>3.2320000000000002</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>300.64999999999998</v>
+        <v>161.6</v>
       </c>
       <c r="F9">
         <v>150</v>
@@ -3340,11 +3340,11 @@
         <v>25</v>
       </c>
       <c r="D10" s="2">
-        <v>2.84</v>
+        <v>1.3180000000000001</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>142</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="F10">
         <v>150</v>
@@ -3361,11 +3361,11 @@
         <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>7.95</v>
+        <v>1.452</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>397.5</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="F11">
         <v>150</v>
@@ -3382,11 +3382,11 @@
         <v>27</v>
       </c>
       <c r="D12" s="2">
-        <v>6.601</v>
+        <v>1.484</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>330.05</v>
+        <v>74.2</v>
       </c>
       <c r="F12">
         <v>150</v>
@@ -3403,11 +3403,11 @@
         <v>31</v>
       </c>
       <c r="D13" s="2">
-        <v>2.9420000000000002</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>147.1</v>
+        <v>51.65</v>
       </c>
       <c r="F13">
         <v>150</v>
@@ -3424,11 +3424,11 @@
         <v>28</v>
       </c>
       <c r="D14" s="2">
-        <v>3.7349999999999999</v>
+        <v>1.4950000000000001</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>186.75</v>
+        <v>74.75</v>
       </c>
       <c r="F14">
         <v>150</v>
@@ -3954,6 +3954,827 @@
       <c r="E39">
         <f t="shared" si="0"/>
         <v>6.4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E4">
+        <f>(D4*1000)/$D$1</f>
+        <v>22.35</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.157</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
+        <v>107.85</v>
+      </c>
+      <c r="F5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>41.55</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.407</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>120.35</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>36.25</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.7370000000000001</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>86.85</v>
+      </c>
+      <c r="F10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.593</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>79.650000000000006</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.83</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>191.5</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>29.55</v>
+      </c>
+      <c r="F13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.661</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>83.05</v>
+      </c>
+      <c r="F14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>73.55</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>120.25</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.316</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>15.8</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.214</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>13.4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>19.3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>8.85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>151.25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>20.45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5.4050000000000002</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>270.25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>5.3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.153</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>7.65</v>
       </c>
       <c r="F39" t="s">
         <v>33</v>
@@ -3973,825 +4794,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="4">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="E4">
-        <f>(D4*1000)/$D$1</f>
-        <v>22.35</v>
-      </c>
-      <c r="F4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.157</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
-        <v>107.85</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>41.55</v>
-      </c>
-      <c r="F6">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.92</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>146</v>
-      </c>
-      <c r="F7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.407</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>120.35</v>
-      </c>
-      <c r="F8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>36.25</v>
-      </c>
-      <c r="F9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.7370000000000001</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>86.85</v>
-      </c>
-      <c r="F10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1.593</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>79.650000000000006</v>
-      </c>
-      <c r="F11">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2">
-        <v>3.83</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>191.5</v>
-      </c>
-      <c r="F12">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.59099999999999997</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>29.55</v>
-      </c>
-      <c r="F13">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1.661</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>83.05</v>
-      </c>
-      <c r="F14">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1.4710000000000001</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>73.55</v>
-      </c>
-      <c r="F15">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2.4049999999999998</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>120.25</v>
-      </c>
-      <c r="F16">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.316</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>15.8</v>
-      </c>
-      <c r="F17">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="2">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>4.2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="2">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.214</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>10.7</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>13.4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>11.5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>19.3</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>8.85</v>
-      </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="2">
-        <v>3.0249999999999999</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>151.25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>20.45</v>
-      </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="2">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="F33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="2">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>1.9</v>
-      </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="2">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="F35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="2">
-        <v>5.4050000000000002</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>270.25</v>
-      </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.106</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>5.3</v>
-      </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>14.25</v>
-      </c>
-      <c r="F38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0.153</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>7.65</v>
-      </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
-      <formula>F4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E39">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>F4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Documented pack 4 with updated parts
</commit_message>
<xml_diff>
--- a/ATPs/ATP-01/01_Accumulator_Verification.xlsx
+++ b/ATPs/ATP-01/01_Accumulator_Verification.xlsx
@@ -3980,7 +3980,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4060,11 +4060,11 @@
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>2.157</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E39" si="0">(D5*1000)/$D$1</f>
-        <v>107.85</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>150</v>
@@ -4081,11 +4081,11 @@
         <v>21</v>
       </c>
       <c r="D6" s="2">
-        <v>0.83099999999999996</v>
+        <v>1.31</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>41.55</v>
+        <v>65.5</v>
       </c>
       <c r="F6">
         <v>150</v>
@@ -4186,11 +4186,11 @@
         <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>1.593</v>
+        <v>1.829</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>79.650000000000006</v>
+        <v>91.45</v>
       </c>
       <c r="F11">
         <v>150</v>
@@ -4207,11 +4207,11 @@
         <v>27</v>
       </c>
       <c r="D12" s="2">
-        <v>3.83</v>
+        <v>2.9279999999999999</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>191.5</v>
+        <v>146.4</v>
       </c>
       <c r="F12">
         <v>150</v>

</xml_diff>

<commit_message>
Updated pack 3 test data
</commit_message>
<xml_diff>
--- a/ATPs/ATP-01/01_Accumulator_Verification.xlsx
+++ b/ATPs/ATP-01/01_Accumulator_Verification.xlsx
@@ -3154,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3277,11 +3277,11 @@
         <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>5.8360000000000003</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>291.8</v>
+        <v>122.5</v>
       </c>
       <c r="F7">
         <v>150</v>
@@ -3298,11 +3298,11 @@
         <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>0.88200000000000001</v>
+        <v>0.623</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>44.1</v>
+        <v>31.15</v>
       </c>
       <c r="F8">
         <v>150</v>
@@ -3319,11 +3319,11 @@
         <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>3.2320000000000002</v>
+        <v>2.1920000000000002</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>161.6</v>
+        <v>109.6</v>
       </c>
       <c r="F9">
         <v>150</v>
@@ -3340,11 +3340,11 @@
         <v>25</v>
       </c>
       <c r="D10" s="2">
-        <v>1.3180000000000001</v>
+        <v>1.9419999999999999</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>65.900000000000006</v>
+        <v>97.1</v>
       </c>
       <c r="F10">
         <v>150</v>

</xml_diff>